<commit_message>
Actualización CU y Tajadas
</commit_message>
<xml_diff>
--- a/Bitacora de Errores/Bitacora de Errores.xlsx
+++ b/Bitacora de Errores/Bitacora de Errores.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace_git\Javeriana\PDCA_Repositorio_Doc\Errores\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\57314\git\PDCA_Repositorio_Doc\Bitacora de Errores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E118B4BA-733B-44BA-A5AA-38AFF1B56BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38EAB6C2-19DA-4895-957A-12D0EFEF3B4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Error</t>
   </si>
@@ -52,6 +52,27 @@
   </si>
   <si>
     <t>Tito Maturanda - Luis Sabroso</t>
+  </si>
+  <si>
+    <t>Se genero error al momento del despleigue an el ajuste de calculo de gastos por pruebas automatizadas no contempladas</t>
+  </si>
+  <si>
+    <t>Se realizo ajuste modificando las pruebas automatizadas para que contemplaran el nuevo campo de gastos</t>
+  </si>
+  <si>
+    <t>Se realiza el ajuste para embeber esta variable para validacion de codigo</t>
+  </si>
+  <si>
+    <t>Se modifico nombre de la clase para no generar warning en la validacion de codigo.</t>
+  </si>
+  <si>
+    <t>Tito Maturanda</t>
+  </si>
+  <si>
+    <t>Se debe generar modificacion del la clase commonDtos por common-dto por validacion de codigo con SpnarQube y Jacoco</t>
+  </si>
+  <si>
+    <t>Se genera error por que la entidad InformacionAportes no tiene InformacionAportesId embebido al momento de adicionar los ajustes para analisis de codigo SonarQube y Jacoco.</t>
   </si>
 </sst>
 </file>
@@ -89,7 +110,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -97,14 +118,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,70 +426,121 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" customWidth="1"/>
-    <col min="3" max="3" width="39.88671875" customWidth="1"/>
-    <col min="4" max="4" width="66.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" customWidth="1"/>
+    <col min="3" max="3" width="39.90625" customWidth="1"/>
+    <col min="4" max="4" width="66.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+    <row r="2" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
         <v>44811</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>44813</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+    <row r="3" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
         <v>44812</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>44813</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>44825</v>
+      </c>
+      <c r="B4" s="2">
+        <v>44825</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>44827</v>
+      </c>
+      <c r="B5" s="2">
+        <v>44827</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>44828</v>
+      </c>
+      <c r="B6" s="2">
+        <v>44828</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>